<commit_message>
battery test three  + calc
</commit_message>
<xml_diff>
--- a/calc-data/batteryData2.xlsx
+++ b/calc-data/batteryData2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="13410" windowHeight="9660"/>
+    <workbookView xWindow="3840" yWindow="0" windowWidth="13410" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10181,11 +10181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97126928"/>
-        <c:axId val="146457392"/>
+        <c:axId val="222121648"/>
+        <c:axId val="222122040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97126928"/>
+        <c:axId val="222121648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10242,12 +10242,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146457392"/>
+        <c:crossAx val="222122040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146457392"/>
+        <c:axId val="222122040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10304,7 +10304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97126928"/>
+        <c:crossAx val="222121648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11209,8 +11209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC3265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11280,7 +11280,7 @@
         <v>476</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H16" si="0">TEXT((INDEX(A$1:A$3600,$G4)-INDEX(A$1:A$3600,$G3)),"mm:ss")</f>
+        <f t="shared" ref="H3:H15" si="0">TEXT((INDEX(A$1:A$3600,$G4)-INDEX(A$1:A$3600,$G3)),"mm:ss")</f>
         <v>14:58</v>
       </c>
       <c r="I3">

</xml_diff>